<commit_message>
Push the some new changes in test case 1 to 5
</commit_message>
<xml_diff>
--- a/testData/testData.xlsx
+++ b/testData/testData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="80">
   <si>
     <t>‘Test Case ID’</t>
   </si>
@@ -54,36 +54,6 @@
     <t>Add a new user in application</t>
   </si>
   <si>
-    <t>1. Launch browser</t>
-  </si>
-  <si>
-    <t>4. Click on 'Signup / Login' button</t>
-  </si>
-  <si>
-    <t>6. Enter name and email address</t>
-  </si>
-  <si>
-    <t>7. Click 'Signup' button</t>
-  </si>
-  <si>
-    <t>9. Fill details: Title, Name, Email, Password, Date of birth</t>
-  </si>
-  <si>
-    <t>10. Select checkbox 'Sign up for our newsletter!'</t>
-  </si>
-  <si>
-    <t>11. Select checkbox 'Receive special offers from our partners!'</t>
-  </si>
-  <si>
-    <t>12. Fill details: First name, Last name, Company, Address, Address2, Country, State, City, Zipcode, Mobile Number</t>
-  </si>
-  <si>
-    <t>13. Click 'Create Account button'</t>
-  </si>
-  <si>
-    <t>15. Click 'Continue' button</t>
-  </si>
-  <si>
     <t>New user must have valid email id</t>
   </si>
   <si>
@@ -138,12 +108,6 @@
     <t>Login in account</t>
   </si>
   <si>
-    <t>6. Enter correct email address and password</t>
-  </si>
-  <si>
-    <t>7. Click 'login' button</t>
-  </si>
-  <si>
     <t>Passed</t>
   </si>
   <si>
@@ -234,9 +198,6 @@
     <t>India</t>
   </si>
   <si>
-    <t>Maha</t>
-  </si>
-  <si>
     <t>June</t>
   </si>
   <si>
@@ -244,6 +205,57 @@
   </si>
   <si>
     <t>nik1@gmail.com</t>
+  </si>
+  <si>
+    <t>Maharashtra</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Launch browser</t>
+  </si>
+  <si>
+    <t>Enter name and email address</t>
+  </si>
+  <si>
+    <t>Click 'Signup' button</t>
+  </si>
+  <si>
+    <t>Fill details: Title, Name, Email, Password, Date of birth</t>
+  </si>
+  <si>
+    <t>Select checkbox 'Sign up for our newsletter!'</t>
+  </si>
+  <si>
+    <t>Select checkbox 'Receive special offers from our partners!'</t>
+  </si>
+  <si>
+    <t>Fill details: First name, Last name, Company, Address, Address2, Country, State, City, Zipcode, Mobile Number</t>
+  </si>
+  <si>
+    <t>Click 'Create Account button'</t>
+  </si>
+  <si>
+    <t>Click 'Continue' button</t>
+  </si>
+  <si>
+    <t>nik2@gmail.com</t>
+  </si>
+  <si>
+    <t>nik3@gmail.com</t>
+  </si>
+  <si>
+    <t>TC0004</t>
+  </si>
+  <si>
+    <t>TC0005</t>
+  </si>
+  <si>
+    <t>TC00014</t>
+  </si>
+  <si>
+    <t>TC00015</t>
+  </si>
+  <si>
+    <t>TC00016</t>
   </si>
 </sst>
 </file>
@@ -726,8 +738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView topLeftCell="E13" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -784,19 +796,19 @@
         <v>11</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -805,7 +817,7 @@
       <c r="C3" s="23"/>
       <c r="D3" s="24"/>
       <c r="E3" s="17" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -814,7 +826,7 @@
       <c r="C4" s="23"/>
       <c r="D4" s="24"/>
       <c r="E4" s="17" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -823,7 +835,7 @@
       <c r="C5" s="23"/>
       <c r="D5" s="24"/>
       <c r="E5" s="17" t="s">
-        <v>15</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -832,7 +844,7 @@
       <c r="C6" s="23"/>
       <c r="D6" s="24"/>
       <c r="E6" s="17" t="s">
-        <v>16</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -841,7 +853,7 @@
       <c r="C7" s="23"/>
       <c r="D7" s="24"/>
       <c r="E7" s="17" t="s">
-        <v>17</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -850,7 +862,7 @@
       <c r="C8" s="23"/>
       <c r="D8" s="24"/>
       <c r="E8" s="17" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -859,7 +871,7 @@
       <c r="C9" s="23"/>
       <c r="D9" s="24"/>
       <c r="E9" s="17" t="s">
-        <v>19</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -868,7 +880,7 @@
       <c r="C10" s="23"/>
       <c r="D10" s="24"/>
       <c r="E10" s="17" t="s">
-        <v>20</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -877,7 +889,7 @@
       <c r="C11" s="23"/>
       <c r="D11" s="24"/>
       <c r="E11" s="17" t="s">
-        <v>21</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -896,49 +908,49 @@
     </row>
     <row r="14" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="G14" s="18" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="7"/>
       <c r="C15" s="6"/>
       <c r="E15" s="17" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="7"/>
       <c r="C16" s="6"/>
       <c r="E16" s="17" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="7"/>
       <c r="C17" s="6"/>
       <c r="E17" s="17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -947,43 +959,43 @@
     </row>
     <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="E19" s="19" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E20" s="19" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E21" s="20" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E22" s="20" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -991,48 +1003,48 @@
     </row>
     <row r="24" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E24" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="G24" s="1" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E25" s="11" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="E26" s="11" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E27" s="11" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E28" s="11" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1049,28 +1061,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.42578125" customWidth="1"/>
     <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.42578125" customWidth="1"/>
     <col min="5" max="5" width="4.28515625" customWidth="1"/>
     <col min="6" max="6" width="7" customWidth="1"/>
-    <col min="7" max="7" width="4.85546875" customWidth="1"/>
+    <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.140625" customWidth="1"/>
-    <col min="9" max="9" width="10" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.28515625" customWidth="1"/>
     <col min="11" max="11" width="8.140625" customWidth="1"/>
     <col min="12" max="12" width="9.140625" customWidth="1"/>
     <col min="13" max="13" width="7.7109375" customWidth="1"/>
-    <col min="14" max="14" width="5.5703125" customWidth="1"/>
+    <col min="14" max="14" width="12" customWidth="1"/>
     <col min="15" max="15" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="8" customWidth="1"/>
     <col min="17" max="17" width="14.85546875" customWidth="1"/>
@@ -1081,52 +1093,52 @@
         <v>0</v>
       </c>
       <c r="B1" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="N1" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="O1" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="P1" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="H1" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="I1" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="J1" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="K1" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="L1" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="M1" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="N1" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="O1" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="P1" s="21" t="s">
-        <v>36</v>
-      </c>
       <c r="Q1" s="21" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -1134,61 +1146,237 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="E2">
         <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="G2">
         <v>1992</v>
       </c>
       <c r="H2" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="I2" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="J2" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="K2" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="L2" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="M2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="N2" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="O2" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="P2">
         <v>441225</v>
       </c>
       <c r="Q2">
         <v>123456789</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
+        <v>60</v>
+      </c>
+      <c r="G7">
+        <v>1992</v>
+      </c>
+      <c r="H7" t="s">
+        <v>55</v>
+      </c>
+      <c r="I7" t="s">
+        <v>56</v>
+      </c>
+      <c r="J7" t="s">
+        <v>57</v>
+      </c>
+      <c r="K7" t="s">
+        <v>58</v>
+      </c>
+      <c r="L7" t="s">
+        <v>58</v>
+      </c>
+      <c r="M7" t="s">
+        <v>59</v>
+      </c>
+      <c r="N7" t="s">
+        <v>63</v>
+      </c>
+      <c r="O7" t="s">
+        <v>58</v>
+      </c>
+      <c r="P7">
+        <v>441225</v>
+      </c>
+      <c r="Q7">
+        <v>123456789</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G8">
+        <v>1992</v>
+      </c>
+      <c r="H8" t="s">
+        <v>55</v>
+      </c>
+      <c r="I8" t="s">
+        <v>56</v>
+      </c>
+      <c r="J8" t="s">
+        <v>57</v>
+      </c>
+      <c r="K8" t="s">
+        <v>58</v>
+      </c>
+      <c r="L8" t="s">
+        <v>58</v>
+      </c>
+      <c r="M8" t="s">
+        <v>59</v>
+      </c>
+      <c r="N8" t="s">
+        <v>63</v>
+      </c>
+      <c r="O8" t="s">
+        <v>58</v>
+      </c>
+      <c r="P8">
+        <v>441225</v>
+      </c>
+      <c r="Q8">
+        <v>123456789</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="C3" r:id="rId3"/>
+    <hyperlink ref="D3" r:id="rId4"/>
+    <hyperlink ref="C4" r:id="rId5"/>
+    <hyperlink ref="D4" r:id="rId6"/>
+    <hyperlink ref="D5" r:id="rId7"/>
+    <hyperlink ref="C6" r:id="rId8"/>
+    <hyperlink ref="C7" r:id="rId9"/>
+    <hyperlink ref="D7" r:id="rId10"/>
+    <hyperlink ref="C8" r:id="rId11"/>
+    <hyperlink ref="D8" r:id="rId12"/>
+    <hyperlink ref="C9" r:id="rId13"/>
+    <hyperlink ref="D9" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId15"/>
 </worksheet>
 </file>
 

</xml_diff>